<commit_message>
complete implement for Statistics. complete the statistics back-end interface. optimize some code.
</commit_message>
<xml_diff>
--- a/backlog&&prototype/backlog3.0.xlsx
+++ b/backlog&&prototype/backlog3.0.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070"/>
+    <workbookView windowWidth="23028" windowHeight="10020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$60</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -580,6 +580,105 @@
     <t>The report about statistics of methods of payment in the last week can be shown.</t>
   </si>
   <si>
+    <t>View Availability</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want to know whether an option is available when ordering,
+so that I can avoid ordering dishes that are not served actually.</t>
+  </si>
+  <si>
+    <t>The availability of each option should be shown on the menu.
+If an option is not available, customers cannot choose it or a popup  dialog is shown.</t>
+  </si>
+  <si>
+    <t>Successful Registeration</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want to receive detailed information printed on the bill after successful registration,
+so that I can avoid fault information.</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>The registration details are printed in the ticket after successful registration.  
+The membership information is written into file.</t>
+  </si>
+  <si>
+    <t>View Information</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want to view individual membership information,
+so that I can identify myself.</t>
+  </si>
+  <si>
+    <t>Customers have access to the personal information interface to view the information entered during registration.</t>
+  </si>
+  <si>
+    <t>Coupons Number</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want to check the number of virtual stamps they have,
+so that I can make the plan to dine there next time.</t>
+  </si>
+  <si>
+    <t>Customers can know the number of their virtual stamps after correctly entering their membership number.</t>
+  </si>
+  <si>
+    <t>Notify Change</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want to be notified by SMS or email each time the number of virtual stamps changes,
+so that I can know the latest number of virtual stamps.</t>
+  </si>
+  <si>
+    <t>After payment, the system queries the contact information of the customer.
+The system sends a message or mail to the customer.</t>
+  </si>
+  <si>
+    <t>Back to Fixed Ramen GUI</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want that the user interface shows the items I have choosed,
+so that I can decide whether to change my options.</t>
+  </si>
+  <si>
+    <t>When customers cliked the "Back" button, the selected options are shown in the fixed Ramen user interface.
+Even though customers do not make any change, "Next" button is available.</t>
+  </si>
+  <si>
+    <t>When customers cliked the "Back" button, the selected options are shown in the add-ons user interface.</t>
+  </si>
+  <si>
+    <t>Cancel the Order as a Member</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want to cancel my order but my stamps do not be set,
+so that there is no loss when cancelling the order.</t>
+  </si>
+  <si>
+    <t>When customers cliked the "Cancel" button, the number of collected stamps does not be subtracted 10.</t>
+  </si>
+  <si>
+    <t>Choose Stamps Use</t>
+  </si>
+  <si>
+    <t>As a customer,
+I want to choose whether to use my stamps to get a discount,
+so that I can make my choices according to my individual situation.</t>
+  </si>
+  <si>
+    <t>When the number of virtual stamps is more than or equal to 10, a popup dialog is shown to ask customers about stamps use.
+If customers do not chooose using stamps, they can pay the bill as usual and get a stamps when successful payment.</t>
+  </si>
+  <si>
     <t>Visualization</t>
   </si>
   <si>
@@ -588,94 +687,7 @@
 so that I can get information intuitively and quickly adjust the business strategy.</t>
   </si>
   <si>
-    <t>medium</t>
-  </si>
-  <si>
     <t>Result shown must be raw data, with no modification.</t>
-  </si>
-  <si>
-    <t>Successful Registeration</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want to receive detailed information printed on the bill after successful registration,
-so that I can avoid fault information.</t>
-  </si>
-  <si>
-    <t>The registration details are printed in the ticket after successful registration.  
-The membership information is written into file.</t>
-  </si>
-  <si>
-    <t>View Information</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want to view individual membership information,
-so that I can identify myself.</t>
-  </si>
-  <si>
-    <t>Customers have access to the personal information interface to view the information entered during registration.</t>
-  </si>
-  <si>
-    <t>Coupons Number</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want to check the number of virtual stamps they have,
-so that I can make the plan to dine there next time.</t>
-  </si>
-  <si>
-    <t>Customers can know the number of their virtual stamps after correctly entering their membership number.</t>
-  </si>
-  <si>
-    <t>Notify Change</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want to be notified by SMS or email each time the number of virtual stamps changes,
-so that I can know the latest number of virtual stamps.</t>
-  </si>
-  <si>
-    <t>After payment, the system queries the contact information of the customer.
-The system sends a message or mail to the customer.</t>
-  </si>
-  <si>
-    <t>Back to Fixed Ramen GUI</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want that the user interface shows the items I have choosed,
-so that I can decide whether to change my options.</t>
-  </si>
-  <si>
-    <t>When customers cliked the "Back" button, the selected options are shown in the fixed Ramen user interface.
-Even though customers do not make any change, "Next" button is available.</t>
-  </si>
-  <si>
-    <t>When customers cliked the "Back" button, the selected options are shown in the add-ons user interface.</t>
-  </si>
-  <si>
-    <t>Cancel the Order as a Member</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want to cancel my order but my stamps do not be set,
-so that there is no loss when cancelling the order.</t>
-  </si>
-  <si>
-    <t>When customers cliked the "Cancel" button, the number of collected stamps does not be subtracted 10.</t>
-  </si>
-  <si>
-    <t>Choose Stamps Use</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want to choose whether to use my stamps to get a discount,
-so that I can make my choices according to my individual situation.</t>
-  </si>
-  <si>
-    <t>When the number of virtual stamps is more than or equal to 10, a popup dialog is shown to ask customers about stamps use.
-If customers do not chooose using stamps, they can pay the bill as usual and get a stamps when successful payment.</t>
   </si>
   <si>
     <t>View Membership Information</t>
@@ -687,18 +699,6 @@
   </si>
   <si>
     <t>The manager has access to the information of members，including the number of members and their virutal stamps.</t>
-  </si>
-  <si>
-    <t>View Availability</t>
-  </si>
-  <si>
-    <t>As a customer,
-I want to know whether an option is available when ordering,
-so that I can avoid ordering dishes that are not served actually.</t>
-  </si>
-  <si>
-    <t>The availability of each option should be shown on the menu.
-If an option is not available, customers cannot choose it or a popup  dialog is shown.</t>
   </si>
   <si>
     <t>More Dishes</t>
@@ -743,9 +743,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -765,7 +765,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -780,30 +834,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -811,21 +849,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -840,38 +863,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -886,23 +893,16 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -923,7 +923,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,7 +1019,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -947,37 +1037,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,7 +1055,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,49 +1073,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,37 +1097,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,25 +1140,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1188,6 +1179,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1202,17 +1208,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1242,10 +1242,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1254,137 +1254,136 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -1404,9 +1403,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1417,9 +1413,6 @@
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1431,54 +1424,91 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1836,1649 +1866,1650 @@
   <sheetPr/>
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A20" sqref="$A20:$XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.13636363636364" style="5" customWidth="1"/>
-    <col min="2" max="2" width="44.5454545454545" style="5" customWidth="1"/>
-    <col min="3" max="3" width="48.9727272727273" customWidth="1"/>
-    <col min="4" max="4" width="13.1090909090909" style="5" customWidth="1"/>
-    <col min="5" max="5" width="28.4272727272727" style="5" customWidth="1"/>
-    <col min="6" max="6" width="38.0909090909091" customWidth="1"/>
-    <col min="7" max="7" width="17.1363636363636" customWidth="1"/>
-    <col min="8" max="8" width="33.6363636363636" customWidth="1"/>
-    <col min="9" max="9" width="30.4909090909091" customWidth="1"/>
+    <col min="1" max="1" width="9.13888888888889" style="4" customWidth="1"/>
+    <col min="2" max="2" width="44.5462962962963" style="4" customWidth="1"/>
+    <col min="3" max="3" width="48.9722222222222" customWidth="1"/>
+    <col min="4" max="4" width="13.1111111111111" style="4" customWidth="1"/>
+    <col min="5" max="5" width="28.4259259259259" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.0925925925926" customWidth="1"/>
+    <col min="7" max="7" width="17.1388888888889" customWidth="1"/>
+    <col min="8" max="8" width="33.6388888888889" customWidth="1"/>
+    <col min="9" max="9" width="30.4907407407407" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="70" spans="1:9">
-      <c r="A2" s="11">
+    <row r="2" s="1" customFormat="1" ht="72" spans="1:9">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="D2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="10">
         <v>1</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16">
+      <c r="G2" s="13"/>
+      <c r="H2" s="14">
         <v>43913</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="14">
         <v>43916</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="91" customHeight="1" spans="1:9">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16">
+      <c r="G3" s="13"/>
+      <c r="H3" s="14">
         <v>43913</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="14">
         <v>43916</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A4" s="11">
+    <row r="4" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16">
+      <c r="G4" s="13"/>
+      <c r="H4" s="14">
         <v>43913</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="14">
         <v>43916</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A5" s="11">
+    <row r="5" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="D5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10">
         <v>1</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16">
+      <c r="G5" s="13"/>
+      <c r="H5" s="14">
         <v>43913</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="14">
         <v>43916</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A6" s="11">
+    <row r="6" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16">
+      <c r="G6" s="13"/>
+      <c r="H6" s="14">
         <v>43913</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="14">
         <v>43916</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A7" s="11">
+    <row r="7" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="D7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10">
         <v>1</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16">
+      <c r="G7" s="13"/>
+      <c r="H7" s="14">
         <v>43913</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="14">
         <v>43916</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="140" spans="1:9">
-      <c r="A8" s="11">
+    <row r="8" s="1" customFormat="1" ht="144" spans="1:9">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="D8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16">
+      <c r="G8" s="13"/>
+      <c r="H8" s="14">
         <v>43913</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="14">
         <v>43916</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" ht="98" spans="1:9">
-      <c r="A9" s="11">
+    <row r="9" s="1" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="D9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="10">
         <v>1</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="16">
+      <c r="G9" s="10"/>
+      <c r="H9" s="14">
         <v>43913</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="14">
         <v>43916</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="70" spans="1:9">
-      <c r="A10" s="11">
+    <row r="10" s="1" customFormat="1" ht="72" spans="1:9">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="D10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="10">
         <v>1</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16">
+      <c r="G10" s="13"/>
+      <c r="H10" s="14">
         <v>43917</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="14">
         <v>43920</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" ht="70" spans="1:9">
-      <c r="A11" s="11">
+    <row r="11" s="1" customFormat="1" ht="72" spans="1:9">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="11">
+      <c r="D11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="10">
         <v>1</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16">
+      <c r="G11" s="13"/>
+      <c r="H11" s="14">
         <v>43917</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="14">
         <v>43920</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" ht="70" spans="1:9">
-      <c r="A12" s="11">
-        <v>11</v>
-      </c>
-      <c r="B12" s="12" t="s">
+    <row r="12" s="1" customFormat="1" ht="72" spans="1:9">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="11">
+      <c r="D12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="10">
         <v>1</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16">
+      <c r="G12" s="13"/>
+      <c r="H12" s="14">
         <v>43917</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="14">
         <v>43920</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" ht="70" spans="1:9">
-      <c r="A13" s="11">
+    <row r="13" s="1" customFormat="1" ht="72" spans="1:9">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="11">
+      <c r="D13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="10">
         <v>1</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16">
+      <c r="G13" s="13"/>
+      <c r="H13" s="14">
         <v>43917</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="14">
         <v>43920</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A14" s="11">
+    <row r="14" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="11">
+      <c r="D14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="10">
         <v>1</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16">
+      <c r="G14" s="13"/>
+      <c r="H14" s="14">
         <v>43917</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="14">
         <v>43920</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A15" s="11">
+    <row r="15" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="11">
+      <c r="D15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="10">
         <v>1</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="16">
+      <c r="G15" s="10"/>
+      <c r="H15" s="14">
         <v>43917</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="14">
         <v>43920</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" ht="126" spans="1:9">
-      <c r="A16" s="11">
+    <row r="16" s="1" customFormat="1" ht="129.6" spans="1:9">
+      <c r="A16" s="10">
         <v>19</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="18">
+      <c r="D16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="15">
         <v>1</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="16">
+      <c r="G16" s="17"/>
+      <c r="H16" s="14">
         <v>43921</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="14">
         <v>43923</v>
       </c>
     </row>
-    <row r="17" s="2" customFormat="1" ht="182" spans="1:9">
-      <c r="A17" s="12">
+    <row r="17" s="1" customFormat="1" ht="187.2" spans="1:9">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="D17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="15">
         <v>2</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23">
+      <c r="G17" s="17"/>
+      <c r="H17" s="14">
         <v>43927</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="14">
         <v>43929</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="115" customHeight="1" spans="1:9">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="18">
+      <c r="D18" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="15">
         <v>2</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="16">
+      <c r="G18" s="17"/>
+      <c r="H18" s="14">
         <v>43929</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="14">
         <v>43932</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="1" ht="140" spans="1:9">
-      <c r="A19" s="11">
+    <row r="19" s="1" customFormat="1" ht="144" spans="1:9">
+      <c r="A19" s="10">
         <v>21</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="18">
+      <c r="D19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="15">
         <v>2</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="16">
+      <c r="G19" s="17"/>
+      <c r="H19" s="14">
         <v>43929</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="14">
         <v>43932</v>
       </c>
     </row>
-    <row r="20" s="1" customFormat="1" ht="168" spans="1:9">
-      <c r="A20" s="11">
+    <row r="20" s="1" customFormat="1" ht="172.8" spans="1:9">
+      <c r="A20" s="10">
         <v>18</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="18">
+      <c r="D20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="15">
         <v>2</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="16">
+      <c r="G20" s="17"/>
+      <c r="H20" s="14">
         <v>43929</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="14">
         <v>43934</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" ht="140" spans="1:9">
-      <c r="A21" s="11">
+    <row r="21" s="1" customFormat="1" ht="144" spans="1:9">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="18">
+      <c r="D21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="15">
         <v>2</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="16">
+      <c r="G21" s="17"/>
+      <c r="H21" s="14">
         <v>43933</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="14">
         <v>43934</v>
       </c>
     </row>
-    <row r="22" s="3" customFormat="1" ht="70" spans="1:9">
-      <c r="A22" s="24">
+    <row r="22" s="2" customFormat="1" ht="72" spans="1:9">
+      <c r="A22" s="19">
         <v>44</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="25">
+      <c r="D22" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="19">
         <v>2</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28">
+      <c r="G22" s="21"/>
+      <c r="H22" s="22">
         <v>43935</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="22">
         <v>43937</v>
       </c>
     </row>
-    <row r="23" s="4" customFormat="1" ht="70" spans="1:9">
-      <c r="A23" s="29">
+    <row r="23" s="3" customFormat="1" ht="72" spans="1:9">
+      <c r="A23" s="23">
         <v>45</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="25">
+      <c r="D23" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="19">
         <v>2</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31">
+      <c r="G23" s="24"/>
+      <c r="H23" s="25">
         <v>43935</v>
       </c>
-      <c r="I23" s="31">
+      <c r="I23" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="24" s="4" customFormat="1" ht="70" spans="1:9">
-      <c r="A24" s="29">
+    <row r="24" s="3" customFormat="1" ht="72" spans="1:9">
+      <c r="A24" s="23">
         <v>46</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="25">
+      <c r="D24" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="19">
         <v>2</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="31">
+      <c r="G24" s="24"/>
+      <c r="H24" s="25">
         <v>43935</v>
       </c>
-      <c r="I24" s="31">
+      <c r="I24" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="25" s="4" customFormat="1" ht="70" spans="1:9">
-      <c r="A25" s="29">
+    <row r="25" s="3" customFormat="1" ht="72" spans="1:9">
+      <c r="A25" s="23">
         <v>47</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="25">
+      <c r="D25" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="19">
         <v>2</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="31">
+      <c r="G25" s="24"/>
+      <c r="H25" s="25">
         <v>43935</v>
       </c>
-      <c r="I25" s="31">
+      <c r="I25" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="26" s="4" customFormat="1" ht="70" spans="1:9">
-      <c r="A26" s="29">
+    <row r="26" s="3" customFormat="1" ht="72" spans="1:9">
+      <c r="A26" s="23">
         <v>48</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="25">
+      <c r="D26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="19">
         <v>2</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="30"/>
-      <c r="H26" s="31">
+      <c r="G26" s="24"/>
+      <c r="H26" s="25">
         <v>43935</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="27" s="4" customFormat="1" ht="98" spans="1:9">
-      <c r="A27" s="29">
+    <row r="27" s="3" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A27" s="23">
         <v>49</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="25">
+      <c r="D27" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="19">
         <v>2</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31">
+      <c r="G27" s="24"/>
+      <c r="H27" s="25">
         <v>43935</v>
       </c>
-      <c r="I27" s="31">
+      <c r="I27" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="28" s="4" customFormat="1" ht="84" spans="1:9">
-      <c r="A28" s="29">
+    <row r="28" s="3" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A28" s="23">
         <v>50</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="25">
+      <c r="D28" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="19">
         <v>2</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="31">
+      <c r="G28" s="24"/>
+      <c r="H28" s="25">
         <v>43935</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="29" s="4" customFormat="1" ht="84" spans="1:9">
-      <c r="A29" s="29">
+    <row r="29" s="3" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A29" s="23">
         <v>51</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="25">
+      <c r="D29" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="19">
         <v>2</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31">
+      <c r="G29" s="24"/>
+      <c r="H29" s="25">
         <v>43935</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="30" s="4" customFormat="1" ht="84" spans="1:9">
-      <c r="A30" s="29">
+    <row r="30" s="3" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A30" s="23">
         <v>52</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="25">
+      <c r="D30" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="19">
         <v>2</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="31">
+      <c r="G30" s="24"/>
+      <c r="H30" s="25">
         <v>43935</v>
       </c>
-      <c r="I30" s="31">
+      <c r="I30" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="31" s="4" customFormat="1" ht="84" spans="1:9">
-      <c r="A31" s="29">
+    <row r="31" s="3" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A31" s="23">
         <v>53</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="25">
+      <c r="D31" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="19">
         <v>2</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="31">
+      <c r="G31" s="24"/>
+      <c r="H31" s="25">
         <v>43935</v>
       </c>
-      <c r="I31" s="31">
+      <c r="I31" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="32" s="4" customFormat="1" ht="84" spans="1:9">
-      <c r="A32" s="29">
+    <row r="32" s="3" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A32" s="23">
         <v>54</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="25">
+      <c r="D32" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="19">
         <v>2</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="31">
+      <c r="G32" s="24"/>
+      <c r="H32" s="25">
         <v>43935</v>
       </c>
-      <c r="I32" s="31">
+      <c r="I32" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="33" s="4" customFormat="1" ht="98" spans="1:9">
-      <c r="A33" s="29">
+    <row r="33" s="3" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A33" s="23">
         <v>55</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="25">
+      <c r="D33" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="19">
         <v>2</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31">
+      <c r="G33" s="24"/>
+      <c r="H33" s="25">
         <v>43935</v>
       </c>
-      <c r="I33" s="31">
+      <c r="I33" s="25">
         <v>43937</v>
       </c>
     </row>
-    <row r="34" customFormat="1" ht="98" spans="1:9">
-      <c r="A34" s="32">
+    <row r="34" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A34" s="26">
         <v>27</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="32">
+      <c r="D34" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="26">
         <v>3</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36">
+      <c r="G34" s="29"/>
+      <c r="H34" s="30">
         <v>43941</v>
       </c>
-      <c r="I34" s="36">
+      <c r="I34" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="35" customFormat="1" ht="98" spans="1:9">
-      <c r="A35" s="32">
+    <row r="35" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A35" s="26">
         <v>28</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="32">
+      <c r="D35" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="26">
         <v>3</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="35"/>
-      <c r="H35" s="36">
+      <c r="G35" s="29"/>
+      <c r="H35" s="30">
         <v>43941</v>
       </c>
-      <c r="I35" s="36">
+      <c r="I35" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="36" customFormat="1" ht="98" spans="1:9">
-      <c r="A36" s="32">
+    <row r="36" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A36" s="26">
         <v>29</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C36" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="32">
+      <c r="D36" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="26">
         <v>3</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="G36" s="35"/>
-      <c r="H36" s="36">
+      <c r="G36" s="29"/>
+      <c r="H36" s="30">
         <v>43941</v>
       </c>
-      <c r="I36" s="36">
+      <c r="I36" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="98" spans="1:9">
-      <c r="A37" s="32">
+    <row r="37" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A37" s="26">
         <v>30</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="32">
+      <c r="D37" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="26">
         <v>3</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="F37" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="36">
+      <c r="G37" s="29"/>
+      <c r="H37" s="30">
         <v>43941</v>
       </c>
-      <c r="I37" s="36">
+      <c r="I37" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="38" customFormat="1" ht="98" spans="1:9">
-      <c r="A38" s="32">
+    <row r="38" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A38" s="26">
         <v>31</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D38" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="32">
+      <c r="D38" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="26">
         <v>3</v>
       </c>
-      <c r="F38" s="34" t="s">
+      <c r="F38" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="36">
+      <c r="G38" s="29"/>
+      <c r="H38" s="30">
         <v>43941</v>
       </c>
-      <c r="I38" s="36">
+      <c r="I38" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="39" customFormat="1" ht="98" spans="1:9">
-      <c r="A39" s="32">
+    <row r="39" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A39" s="26">
         <v>32</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D39" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="32">
+      <c r="D39" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="26">
         <v>3</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="G39" s="35"/>
-      <c r="H39" s="36">
+      <c r="G39" s="29"/>
+      <c r="H39" s="30">
         <v>43941</v>
       </c>
-      <c r="I39" s="36">
+      <c r="I39" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" customFormat="1" ht="98" spans="1:9">
-      <c r="A40" s="32">
+    <row r="40" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A40" s="26">
         <v>33</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="32">
+      <c r="D40" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="26">
         <v>3</v>
       </c>
-      <c r="F40" s="34" t="s">
+      <c r="F40" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G40" s="35"/>
-      <c r="H40" s="36">
+      <c r="G40" s="29"/>
+      <c r="H40" s="30">
         <v>43941</v>
       </c>
-      <c r="I40" s="36">
+      <c r="I40" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="41" customFormat="1" ht="98" spans="1:9">
-      <c r="A41" s="32">
+    <row r="41" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A41" s="26">
         <v>34</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="32">
+      <c r="D41" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="26">
         <v>3</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="F41" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="G41" s="35"/>
-      <c r="H41" s="36">
+      <c r="G41" s="29"/>
+      <c r="H41" s="30">
         <v>43941</v>
       </c>
-      <c r="I41" s="36">
+      <c r="I41" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="42" customFormat="1" ht="112" spans="1:9">
-      <c r="A42" s="32">
+    <row r="42" customFormat="1" ht="115.2" spans="1:9">
+      <c r="A42" s="26">
         <v>35</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="33" t="s">
+      <c r="C42" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="32">
+      <c r="D42" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="26">
         <v>3</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F42" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="G42" s="35"/>
-      <c r="H42" s="36">
+      <c r="G42" s="29"/>
+      <c r="H42" s="30">
         <v>43941</v>
       </c>
-      <c r="I42" s="36">
+      <c r="I42" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="43" customFormat="1" ht="98" spans="1:9">
-      <c r="A43" s="32">
+    <row r="43" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A43" s="26">
         <v>36</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="32">
+      <c r="D43" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="26">
         <v>3</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="F43" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="G43" s="35"/>
-      <c r="H43" s="36">
+      <c r="G43" s="29"/>
+      <c r="H43" s="30">
         <v>43941</v>
       </c>
-      <c r="I43" s="36">
+      <c r="I43" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="44" customFormat="1" ht="98" spans="1:9">
-      <c r="A44" s="32">
+    <row r="44" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A44" s="26">
         <v>37</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="D44" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="32">
+      <c r="D44" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="26">
         <v>3</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F44" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="G44" s="35"/>
-      <c r="H44" s="36">
+      <c r="G44" s="29"/>
+      <c r="H44" s="30">
         <v>43941</v>
       </c>
-      <c r="I44" s="36">
+      <c r="I44" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="45" customFormat="1" ht="98" spans="1:9">
-      <c r="A45" s="32">
+    <row r="45" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A45" s="26">
         <v>38</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="32">
+      <c r="D45" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="26">
         <v>3</v>
       </c>
-      <c r="F45" s="34" t="s">
+      <c r="F45" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="G45" s="35"/>
-      <c r="H45" s="36">
+      <c r="G45" s="29"/>
+      <c r="H45" s="30">
         <v>43941</v>
       </c>
-      <c r="I45" s="36">
+      <c r="I45" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="46" customFormat="1" ht="112" spans="1:9">
-      <c r="A46" s="32">
+    <row r="46" customFormat="1" ht="115.2" spans="1:9">
+      <c r="A46" s="26">
         <v>39</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C46" s="33" t="s">
+      <c r="C46" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="32">
+      <c r="D46" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="26">
         <v>3</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="F46" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="G46" s="35"/>
-      <c r="H46" s="36">
+      <c r="G46" s="29"/>
+      <c r="H46" s="30">
         <v>43941</v>
       </c>
-      <c r="I46" s="36">
+      <c r="I46" s="30">
         <v>43946</v>
       </c>
     </row>
-    <row r="47" customFormat="1" ht="112" spans="1:9">
-      <c r="A47" s="32">
+    <row r="47" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A47" s="33">
+        <v>15</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="33">
+        <v>3</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" s="37"/>
+      <c r="H47" s="38">
+        <v>43957</v>
+      </c>
+      <c r="I47" s="38">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A48" s="39">
+        <v>40</v>
+      </c>
+      <c r="B48" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="42">
+        <v>3</v>
+      </c>
+      <c r="F48" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="G48" s="43"/>
+      <c r="H48" s="44">
+        <v>43947</v>
+      </c>
+      <c r="I48" s="44">
+        <v>43948</v>
+      </c>
+    </row>
+    <row r="49" s="1" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A49" s="39">
+        <v>22</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" s="42">
+        <v>3</v>
+      </c>
+      <c r="F49" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="G49" s="46"/>
+      <c r="H49" s="44">
+        <v>43949</v>
+      </c>
+      <c r="I49" s="44">
+        <v>43951</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A50" s="39">
+        <v>23</v>
+      </c>
+      <c r="B50" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E50" s="42">
+        <v>3</v>
+      </c>
+      <c r="F50" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="G50" s="43"/>
+      <c r="H50" s="44">
+        <v>43949</v>
+      </c>
+      <c r="I50" s="44">
+        <v>43951</v>
+      </c>
+    </row>
+    <row r="51" s="1" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A51" s="39">
+        <v>41</v>
+      </c>
+      <c r="B51" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E51" s="42">
+        <v>3</v>
+      </c>
+      <c r="F51" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="G51" s="43"/>
+      <c r="H51" s="44">
+        <v>43949</v>
+      </c>
+      <c r="I51" s="44">
+        <v>43951</v>
+      </c>
+    </row>
+    <row r="52" s="1" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A52" s="39">
+        <v>56</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E52" s="42">
+        <v>3</v>
+      </c>
+      <c r="F52" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="G52" s="43"/>
+      <c r="H52" s="44">
+        <v>43963</v>
+      </c>
+      <c r="I52" s="44">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="53" s="1" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A53" s="39">
+        <v>57</v>
+      </c>
+      <c r="B53" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="42">
+        <v>3</v>
+      </c>
+      <c r="F53" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="G53" s="43"/>
+      <c r="H53" s="44">
+        <v>43963</v>
+      </c>
+      <c r="I53" s="44">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="54" s="1" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A54" s="39">
+        <v>57</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="42">
+        <v>3</v>
+      </c>
+      <c r="F54" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" s="43"/>
+      <c r="H54" s="44">
+        <v>43963</v>
+      </c>
+      <c r="I54" s="44">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="55" s="1" customFormat="1" ht="129.6" spans="1:9">
+      <c r="A55" s="39">
+        <v>57</v>
+      </c>
+      <c r="B55" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55" s="42">
+        <v>3</v>
+      </c>
+      <c r="F55" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="G55" s="43"/>
+      <c r="H55" s="44">
+        <v>43963</v>
+      </c>
+      <c r="I55" s="44">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="56" customFormat="1" ht="115.2" spans="1:9">
+      <c r="A56" s="33">
         <v>42</v>
       </c>
-      <c r="B47" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" s="32">
-        <v>3</v>
-      </c>
-      <c r="F47" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="G47" s="35"/>
-      <c r="H47" s="36">
+      <c r="B56" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" s="33">
+        <v>4</v>
+      </c>
+      <c r="F56" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="G56" s="37"/>
+      <c r="H56" s="38">
         <v>43941</v>
       </c>
-      <c r="I47" s="36">
+      <c r="I56" s="38">
         <v>43946</v>
       </c>
     </row>
-    <row r="48" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A48" s="11">
-        <v>40</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C48" s="39" t="s">
+    <row r="57" customFormat="1" ht="72" spans="1:9">
+      <c r="A57" s="33">
+        <v>24</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="D48" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E48" s="18">
-        <v>3</v>
-      </c>
-      <c r="F48" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="G48" s="20"/>
-      <c r="H48" s="16">
-        <v>43947</v>
-      </c>
-      <c r="I48" s="16">
-        <v>43948</v>
-      </c>
-    </row>
-    <row r="49" s="1" customFormat="1" ht="84" spans="1:9">
-      <c r="A49" s="11">
-        <v>22</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E49" s="18">
-        <v>3</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="G49" s="15"/>
-      <c r="H49" s="16">
-        <v>43949</v>
-      </c>
-      <c r="I49" s="16">
-        <v>43951</v>
-      </c>
-    </row>
-    <row r="50" s="1" customFormat="1" ht="98" spans="1:9">
-      <c r="A50" s="11">
-        <v>23</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C50" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E50" s="18">
-        <v>3</v>
-      </c>
-      <c r="F50" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="16">
-        <v>43949</v>
-      </c>
-      <c r="I50" s="16">
-        <v>43951</v>
-      </c>
-    </row>
-    <row r="51" s="1" customFormat="1" ht="98" spans="1:9">
-      <c r="A51" s="11">
-        <v>41</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="C51" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D51" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E51" s="18">
-        <v>3</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="16">
-        <v>43949</v>
-      </c>
-      <c r="I51" s="16">
-        <v>43951</v>
-      </c>
-    </row>
-    <row r="52" s="2" customFormat="1" ht="98" spans="1:9">
-      <c r="A52" s="12">
-        <v>56</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="18">
-        <v>3</v>
-      </c>
-      <c r="F52" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="G52" s="22"/>
-      <c r="H52" s="23">
+      <c r="E57" s="50">
+        <v>4</v>
+      </c>
+      <c r="F57" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="G57" s="37"/>
+      <c r="H57" s="38">
+        <v>43955</v>
+      </c>
+      <c r="I57" s="38">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="58" customFormat="1" ht="86.4" spans="1:9">
+      <c r="A58" s="33">
+        <v>26</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="E58" s="33">
+        <v>4</v>
+      </c>
+      <c r="F58" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="G58" s="34"/>
+      <c r="H58" s="51">
+        <v>43957</v>
+      </c>
+      <c r="I58" s="51">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="59" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A59" s="33">
+        <v>25</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="C59" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="E59" s="50">
+        <v>4</v>
+      </c>
+      <c r="F59" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="G59" s="37"/>
+      <c r="H59" s="38">
+        <v>43961</v>
+      </c>
+      <c r="I59" s="38">
+        <v>43962</v>
+      </c>
+    </row>
+    <row r="60" customFormat="1" ht="100.8" spans="1:9">
+      <c r="A60" s="33">
+        <v>43</v>
+      </c>
+      <c r="B60" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="D60" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="E60" s="33">
+        <v>4</v>
+      </c>
+      <c r="F60" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="G60" s="37"/>
+      <c r="H60" s="38">
         <v>43963</v>
       </c>
-      <c r="I52" s="23">
+      <c r="I60" s="38">
         <v>43965</v>
       </c>
     </row>
-    <row r="53" s="2" customFormat="1" ht="98" spans="1:9">
-      <c r="A53" s="12">
-        <v>57</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E53" s="18">
-        <v>3</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="G53" s="22"/>
-      <c r="H53" s="23">
-        <v>43963</v>
-      </c>
-      <c r="I53" s="23">
-        <v>43965</v>
-      </c>
-    </row>
-    <row r="54" s="2" customFormat="1" ht="98" spans="1:9">
-      <c r="A54" s="12">
-        <v>57</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E54" s="18">
-        <v>3</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="G54" s="22"/>
-      <c r="H54" s="23">
-        <v>43963</v>
-      </c>
-      <c r="I54" s="23">
-        <v>43965</v>
-      </c>
-    </row>
-    <row r="55" s="2" customFormat="1" ht="126" spans="1:9">
-      <c r="A55" s="12">
-        <v>57</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E55" s="18">
-        <v>3</v>
-      </c>
-      <c r="F55" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="G55" s="22"/>
-      <c r="H55" s="23">
-        <v>43963</v>
-      </c>
-      <c r="I55" s="23">
-        <v>43965</v>
-      </c>
-    </row>
-    <row r="56" customFormat="1" ht="70" spans="1:9">
-      <c r="A56" s="32">
-        <v>24</v>
-      </c>
-      <c r="B56" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="D56" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="E56" s="25">
-        <v>4</v>
-      </c>
-      <c r="F56" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="G56" s="35"/>
-      <c r="H56" s="36">
-        <v>43955</v>
-      </c>
-      <c r="I56" s="36">
-        <v>43956</v>
-      </c>
-    </row>
-    <row r="57" customFormat="1" ht="98" spans="1:9">
-      <c r="A57" s="32">
-        <v>15</v>
-      </c>
-      <c r="B57" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="E57" s="32">
-        <v>4</v>
-      </c>
-      <c r="F57" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="G57" s="35"/>
-      <c r="H57" s="36">
-        <v>43957</v>
-      </c>
-      <c r="I57" s="36">
-        <v>43960</v>
-      </c>
-    </row>
-    <row r="58" customFormat="1" ht="84" spans="1:9">
-      <c r="A58" s="32">
-        <v>26</v>
-      </c>
-      <c r="B58" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="C58" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="D58" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="E58" s="32">
-        <v>4</v>
-      </c>
-      <c r="F58" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="G58" s="33"/>
-      <c r="H58" s="41">
-        <v>43957</v>
-      </c>
-      <c r="I58" s="41">
-        <v>43960</v>
-      </c>
-    </row>
-    <row r="59" customFormat="1" ht="98" spans="1:9">
-      <c r="A59" s="32">
-        <v>25</v>
-      </c>
-      <c r="B59" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="C59" s="42" t="s">
-        <v>182</v>
-      </c>
-      <c r="D59" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="E59" s="25">
-        <v>4</v>
-      </c>
-      <c r="F59" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="G59" s="35"/>
-      <c r="H59" s="36">
-        <v>43961</v>
-      </c>
-      <c r="I59" s="36">
-        <v>43962</v>
-      </c>
-    </row>
-    <row r="60" customFormat="1" ht="98" spans="1:9">
-      <c r="A60" s="32">
-        <v>43</v>
-      </c>
-      <c r="B60" s="32" t="s">
-        <v>184</v>
-      </c>
-      <c r="C60" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="E60" s="32">
-        <v>4</v>
-      </c>
-      <c r="F60" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="G60" s="35"/>
-      <c r="H60" s="36">
-        <v>43963</v>
-      </c>
-      <c r="I60" s="36">
-        <v>43965</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I55">
-    <sortState ref="A1:I55">
-      <sortCondition ref="E1"/>
+  <autoFilter ref="A1:I60">
+    <sortState ref="A2:I60">
+      <sortCondition ref="E2:E60"/>
+      <sortCondition ref="D2:D60" customList="very high, high, medium, low, very low"/>
     </sortState>
     <extLst/>
   </autoFilter>

</xml_diff>